<commit_message>
Initial manual test case
</commit_message>
<xml_diff>
--- a/ManualTest/guru99 bank.xlsx
+++ b/ManualTest/guru99 bank.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feranmi\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feranmi\python\guru99\ManualTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE3E694-8C86-4128-97C2-70EBD4B08333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F99542A-2E6F-4CBE-91BE-B588621E149D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{6318454C-6C68-4D70-8E55-0D6116439F04}"/>
   </bookViews>
@@ -292,14 +292,14 @@
     <t>Create savings account with valid customer id and valid initial cost</t>
   </si>
   <si>
-    <t>Customer id: 8494393846
-Initial deposite: 500, 502</t>
-  </si>
-  <si>
     <t>Input customer id
 Input initial deposite
 Select current account type
 Click submit button</t>
+  </si>
+  <si>
+    <t>Customer id: 8494393846
+Initial deposite: 500, 503</t>
   </si>
 </sst>
 </file>
@@ -392,19 +392,19 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -799,7 +799,7 @@
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:C30"/>
+      <selection activeCell="F56" sqref="F56:F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -843,355 +843,355 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="11" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="14"/>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="10"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="14"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="11"/>
       <c r="F4" s="14"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="10"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="11"/>
       <c r="F5" s="14"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="11"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="8"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="11"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="11"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="13"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="11"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="11"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="11"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="10" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="13"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="11"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="13"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="11"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="13"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="11"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="13"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="10" t="s">
+      <c r="B18" s="9"/>
+      <c r="C18" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="12"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="12"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="12"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="12"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="9"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="10" t="s">
+      <c r="B22" s="9"/>
+      <c r="C22" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="12"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="9"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="12"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="11"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="12"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="12"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="9"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="10" t="s">
         <v>62</v>
       </c>
       <c r="F27" s="8" t="s">
@@ -1205,7 +1205,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="8"/>
-      <c r="B28" s="12"/>
+      <c r="B28" s="9"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
@@ -1216,7 +1216,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="8"/>
-      <c r="B29" s="12"/>
+      <c r="B29" s="9"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
@@ -1227,7 +1227,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="8"/>
-      <c r="B30" s="12"/>
+      <c r="B30" s="9"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
@@ -1240,17 +1240,17 @@
       <c r="A31" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="9" t="s">
+      <c r="B31" s="9"/>
+      <c r="C31" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F31" s="10" t="s">
         <v>59</v>
       </c>
       <c r="G31" s="8" t="s">
@@ -1261,8 +1261,8 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="8"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="10"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
@@ -1272,8 +1272,8 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="8"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="10"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
@@ -1283,8 +1283,8 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="8"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="10"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
@@ -1296,17 +1296,17 @@
       <c r="A35" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="9" t="s">
+      <c r="B35" s="9"/>
+      <c r="C35" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="F35" s="10" t="s">
         <v>60</v>
       </c>
       <c r="G35" s="8" t="s">
@@ -1317,8 +1317,8 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="8"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="10"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
@@ -1328,8 +1328,8 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="8"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="10"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
@@ -1339,8 +1339,8 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="8"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="10"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
@@ -1352,17 +1352,17 @@
       <c r="A39" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="9" t="s">
+      <c r="B39" s="9"/>
+      <c r="C39" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D39" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E39" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F39" s="9" t="s">
+      <c r="F39" s="10" t="s">
         <v>64</v>
       </c>
       <c r="G39" s="8" t="s">
@@ -1373,8 +1373,8 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="8"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="10"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
@@ -1384,8 +1384,8 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="8"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="10"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
@@ -1395,8 +1395,8 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="8"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="10"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
@@ -1408,17 +1408,17 @@
       <c r="A43" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="12"/>
-      <c r="C43" s="9" t="s">
+      <c r="B43" s="9"/>
+      <c r="C43" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D43" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="F43" s="10" t="s">
         <v>63</v>
       </c>
       <c r="G43" s="8" t="s">
@@ -1429,8 +1429,8 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="8"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="10"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
@@ -1440,8 +1440,8 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="8"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="10"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
@@ -1451,8 +1451,8 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="8"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="10"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
@@ -1464,17 +1464,17 @@
       <c r="A47" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B47" s="12"/>
-      <c r="C47" s="9" t="s">
+      <c r="B47" s="9"/>
+      <c r="C47" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D47" s="9" t="s">
+      <c r="D47" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="E47" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F47" s="9" t="s">
+      <c r="F47" s="10" t="s">
         <v>71</v>
       </c>
       <c r="G47" s="8" t="s">
@@ -1483,8 +1483,8 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="8"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="10"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
@@ -1492,8 +1492,8 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="8"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="10"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
@@ -1501,8 +1501,8 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="8"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="10"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
@@ -1512,19 +1512,19 @@
       <c r="A52" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D52" s="9" t="s">
+      <c r="D52" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E52" s="9" t="s">
+      <c r="E52" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F52" s="9" t="s">
+      <c r="F52" s="10" t="s">
         <v>73</v>
       </c>
       <c r="G52" s="8" t="s">
@@ -1533,8 +1533,8 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="8"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="10"/>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
@@ -1542,8 +1542,8 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="8"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="10"/>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
@@ -1551,8 +1551,8 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="8"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="10"/>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
@@ -1562,18 +1562,18 @@
       <c r="A56" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B56" s="12"/>
-      <c r="C56" s="9" t="s">
+      <c r="B56" s="9"/>
+      <c r="C56" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D56" s="9" t="s">
+      <c r="D56" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E56" s="9" t="s">
+      <c r="E56" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F56" s="10" t="s">
         <v>77</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="G56" s="8" t="s">
         <v>66</v>
@@ -1581,8 +1581,8 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="8"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="10"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
@@ -1590,8 +1590,8 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="8"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="10"/>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
@@ -1599,8 +1599,8 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="8"/>
-      <c r="B59" s="12"/>
-      <c r="C59" s="9"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="10"/>
       <c r="D59" s="8"/>
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
@@ -1608,6 +1608,91 @@
     </row>
   </sheetData>
   <mergeCells count="109">
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="H27:H30"/>
+    <mergeCell ref="I27:I30"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="D35:D38"/>
+    <mergeCell ref="F31:F34"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="H31:H34"/>
+    <mergeCell ref="H35:H38"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="I22:I25"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="I6:I9"/>
+    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="I14:I17"/>
+    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="B2:B25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="D39:D42"/>
+    <mergeCell ref="D43:D46"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="E43:E46"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="H39:H42"/>
+    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="I31:I34"/>
+    <mergeCell ref="I35:I38"/>
+    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="I43:I46"/>
+    <mergeCell ref="F39:F42"/>
+    <mergeCell ref="F43:F46"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="G35:G38"/>
+    <mergeCell ref="G39:G42"/>
+    <mergeCell ref="G43:G46"/>
     <mergeCell ref="A56:A59"/>
     <mergeCell ref="B27:B50"/>
     <mergeCell ref="C56:C59"/>
@@ -1632,91 +1717,6 @@
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="A35:A38"/>
     <mergeCell ref="A39:A42"/>
-    <mergeCell ref="H39:H42"/>
-    <mergeCell ref="H43:H46"/>
-    <mergeCell ref="I31:I34"/>
-    <mergeCell ref="I35:I38"/>
-    <mergeCell ref="I39:I42"/>
-    <mergeCell ref="I43:I46"/>
-    <mergeCell ref="F39:F42"/>
-    <mergeCell ref="F43:F46"/>
-    <mergeCell ref="G31:G34"/>
-    <mergeCell ref="G35:G38"/>
-    <mergeCell ref="G39:G42"/>
-    <mergeCell ref="G43:G46"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="B2:B25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C43:C46"/>
-    <mergeCell ref="D39:D42"/>
-    <mergeCell ref="D43:D46"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="E43:E46"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="I22:I25"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="I6:I9"/>
-    <mergeCell ref="I10:I13"/>
-    <mergeCell ref="I14:I17"/>
-    <mergeCell ref="I18:I21"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="H27:H30"/>
-    <mergeCell ref="I27:I30"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="D35:D38"/>
-    <mergeCell ref="F31:F34"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="F35:F38"/>
-    <mergeCell ref="H31:H34"/>
-    <mergeCell ref="H35:H38"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="E35:E38"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>